<commit_message>
feat: implement AI chat system with bug fixes
- Add complete AI orchestration system with chat API
- Implement session management and context retention
- Add PDF generation and email simulation services
- Create enhanced chat UI with proper markdown rendering
- Fix session context message repetition issue
- Add clickable PDF download links with proper URLs
- Implement email confirmation Y/N flow
- Add comprehensive test suite

🤖 Generated with Claude Code

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/MiLA/data/sample_loans.xlsx
+++ b/MiLA/data/sample_loans.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Loans" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -429,20 +429,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="23" customWidth="1" min="2" max="2"/>
-    <col width="19" customWidth="1" min="3" max="3"/>
-    <col width="22" customWidth="1" min="4" max="4"/>
-    <col width="21" customWidth="1" min="5" max="5"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
@@ -470,12 +463,15 @@
           <t>Last Payment Date</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Email Address</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>69253358</t>
-        </is>
+      <c r="A2" t="n">
+        <v>69253358</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -491,12 +487,15 @@
       <c r="E2" s="2" t="n">
         <v>45820</v>
       </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>mark.wilson@email.com</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>8321619</t>
-        </is>
+      <c r="A3" t="n">
+        <v>8321619</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -512,12 +511,15 @@
       <c r="E3" s="2" t="n">
         <v>45813</v>
       </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>david.lewis@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>30036714</t>
-        </is>
+      <c r="A4" t="n">
+        <v>30036714</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -533,12 +535,15 @@
       <c r="E4" s="2" t="n">
         <v>45560</v>
       </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>lisa.garcia@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>12044751</t>
-        </is>
+      <c r="A5" t="n">
+        <v>12044751</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -554,12 +559,15 @@
       <c r="E5" s="2" t="n">
         <v>45635</v>
       </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>daniel.perez@yahoo.com</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>16390386</t>
-        </is>
+      <c r="A6" t="n">
+        <v>16390386</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -575,12 +583,15 @@
       <c r="E6" s="2" t="n">
         <v>45719</v>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>sarah.sanchez@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>18391162</t>
-        </is>
+      <c r="A7" t="n">
+        <v>18391162</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -596,12 +607,15 @@
       <c r="E7" s="2" t="n">
         <v>45740</v>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>amanda.brown@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>92623870</t>
-        </is>
+      <c r="A8" t="n">
+        <v>92623870</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -617,12 +631,15 @@
       <c r="E8" s="2" t="n">
         <v>45870</v>
       </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>emma.gonzalez@outlook.com</t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>27145700</t>
-        </is>
+      <c r="A9" t="n">
+        <v>27145700</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -638,12 +655,15 @@
       <c r="E9" s="2" t="n">
         <v>45621</v>
       </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>michelle.lee@email.com</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>13361992</t>
-        </is>
+      <c r="A10" t="n">
+        <v>13361992</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -659,12 +679,15 @@
       <c r="E10" s="2" t="n">
         <v>45801</v>
       </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>james.jones@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>9437188</t>
-        </is>
+      <c r="A11" t="n">
+        <v>9437188</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -680,12 +703,15 @@
       <c r="E11" s="2" t="n">
         <v>45662</v>
       </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>christopher.lewis@email.com</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>46404179</t>
-        </is>
+      <c r="A12" t="n">
+        <v>46404179</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -701,12 +727,15 @@
       <c r="E12" s="2" t="n">
         <v>45727</v>
       </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>sarah.thomas@email.com</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>54424579</t>
-        </is>
+      <c r="A13" t="n">
+        <v>54424579</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -722,12 +751,15 @@
       <c r="E13" s="2" t="n">
         <v>45714</v>
       </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>donald.robinson@yahoo.com</t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>22066387</t>
-        </is>
+      <c r="A14" t="n">
+        <v>22066387</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -743,12 +775,15 @@
       <c r="E14" s="2" t="n">
         <v>45733</v>
       </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>william.clark@yahoo.com</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>36180738</t>
-        </is>
+      <c r="A15" t="n">
+        <v>36180738</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -764,12 +799,15 @@
       <c r="E15" s="2" t="n">
         <v>45700</v>
       </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>emily.anderson@outlook.com</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>61418762</t>
-        </is>
+      <c r="A16" t="n">
+        <v>61418762</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -785,12 +823,15 @@
       <c r="E16" s="2" t="n">
         <v>45779</v>
       </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>emma.ramirez@outlook.com</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>2380001</t>
-        </is>
+      <c r="A17" t="n">
+        <v>2380001</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -806,12 +847,15 @@
       <c r="E17" s="2" t="n">
         <v>45856</v>
       </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>christopher.hernandez@outlook.com</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>793683</t>
-        </is>
+      <c r="A18" t="n">
+        <v>793683</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -827,12 +871,15 @@
       <c r="E18" s="2" t="n">
         <v>45850</v>
       </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>angela.clark@email.com</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>75484401</t>
-        </is>
+      <c r="A19" t="n">
+        <v>75484401</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -848,12 +895,15 @@
       <c r="E19" s="2" t="n">
         <v>45655</v>
       </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>david.thompson@email.com</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>11667225</t>
-        </is>
+      <c r="A20" t="n">
+        <v>11667225</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -869,12 +919,15 @@
       <c r="E20" s="2" t="n">
         <v>45837</v>
       </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>donald.davis@gmail.com</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>17388224</t>
-        </is>
+      <c r="A21" t="n">
+        <v>17388224</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -889,6 +942,11 @@
       </c>
       <c r="E21" s="2" t="n">
         <v>45829</v>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>stephanie.lewis@yahoo.com</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>